<commit_message>
Add splitting for TripleMu seed for Tau3mu search
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_3_0_forEfe/PrescaleTable/L1Menu_Collisions2022_v1_3_0_forEfe.xlsx
+++ b/development/L1Menu_Collisions2022_v1_3_0_forEfe/PrescaleTable/L1Menu_Collisions2022_v1_3_0_forEfe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_3_0_forEfe/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7AA548-4FBE-4045-A558-B0C4652898CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196D86CC-EDDC-274F-955F-418BA6E6EA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="-18780" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="422">
   <si>
     <t>Index</t>
   </si>
@@ -1105,9 +1105,6 @@
     <t>L1_SingleJet43er2p5_NotBptxOR_3BX</t>
   </si>
   <si>
-    <t>L1_SingleJet46er2p5_NotBptxOR_3BX</t>
-  </si>
-  <si>
     <t>L1_AlwaysTrue</t>
   </si>
   <si>
@@ -1280,6 +1277,15 @@
   </si>
   <si>
     <t>L1_DoubleMu_12_5_EMTF</t>
+  </si>
+  <si>
+    <t>L1_TripleMu_2SQ_1p5SQ_0OQ_Mass_Max12_BMTF</t>
+  </si>
+  <si>
+    <t>L1_TripleMu_2SQ_1p5SQ_0OQ_Mass_Max12_OMTF</t>
+  </si>
+  <si>
+    <t>L1_TripleMu_2SQ_1p5SQ_0OQ_Mass_Max12_EMTF</t>
   </si>
 </sst>
 </file>
@@ -1665,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K410"/>
+  <dimension ref="A1:K412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="B391" sqref="B391"/>
+    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5776,7 +5782,7 @@
         <v>127</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C118" s="3">
         <v>0</v>
@@ -6126,7 +6132,7 @@
         <v>141</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C128" s="3">
         <v>0</v>
@@ -6161,7 +6167,7 @@
         <v>142</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C129" s="3">
         <v>0</v>
@@ -6231,7 +6237,7 @@
         <v>144</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C131" s="3">
         <v>0</v>
@@ -6266,7 +6272,7 @@
         <v>145</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C132" s="3">
         <v>0</v>
@@ -11516,7 +11522,7 @@
         <v>334</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C282" s="3">
         <v>0</v>
@@ -11551,7 +11557,7 @@
         <v>335</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C283" s="3">
         <v>0</v>
@@ -13546,7 +13552,7 @@
         <v>418</v>
       </c>
       <c r="B340" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C340">
         <v>0</v>
@@ -13581,7 +13587,7 @@
         <v>419</v>
       </c>
       <c r="B341" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C341">
         <v>0</v>
@@ -13616,7 +13622,7 @@
         <v>420</v>
       </c>
       <c r="B342" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C342">
         <v>0</v>
@@ -13861,7 +13867,7 @@
         <v>427</v>
       </c>
       <c r="B349" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C349">
         <v>0</v>
@@ -13896,7 +13902,7 @@
         <v>428</v>
       </c>
       <c r="B350" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C350">
         <v>0</v>
@@ -14381,117 +14387,117 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A364">
-        <v>454</v>
-      </c>
-      <c r="B364" t="s">
-        <v>361</v>
-      </c>
-      <c r="C364">
-        <v>0</v>
-      </c>
-      <c r="D364">
-        <v>0</v>
-      </c>
-      <c r="E364">
-        <v>0</v>
-      </c>
-      <c r="F364">
-        <v>0</v>
-      </c>
-      <c r="G364">
-        <v>0</v>
-      </c>
-      <c r="H364">
-        <v>0</v>
-      </c>
-      <c r="I364">
-        <v>0</v>
-      </c>
-      <c r="J364">
-        <v>0</v>
-      </c>
-      <c r="K364">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A365">
-        <v>458</v>
-      </c>
-      <c r="B365" t="s">
-        <v>362</v>
-      </c>
-      <c r="C365">
-        <v>0</v>
-      </c>
-      <c r="D365">
-        <v>0</v>
-      </c>
-      <c r="E365">
-        <v>0</v>
-      </c>
-      <c r="F365">
-        <v>0</v>
-      </c>
-      <c r="G365">
-        <v>0</v>
-      </c>
-      <c r="H365">
-        <v>0</v>
-      </c>
-      <c r="I365">
-        <v>0</v>
-      </c>
-      <c r="J365">
-        <v>0</v>
-      </c>
-      <c r="K365">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A366">
-        <v>459</v>
-      </c>
-      <c r="B366" t="s">
-        <v>363</v>
-      </c>
-      <c r="C366">
-        <v>17881</v>
-      </c>
-      <c r="D366">
-        <v>17881</v>
-      </c>
-      <c r="E366">
-        <v>17881</v>
-      </c>
-      <c r="F366">
-        <v>17881</v>
-      </c>
-      <c r="G366">
-        <v>17881</v>
-      </c>
-      <c r="H366">
-        <v>17881</v>
-      </c>
-      <c r="I366">
-        <v>17881</v>
-      </c>
-      <c r="J366">
-        <v>17881</v>
-      </c>
-      <c r="K366">
-        <v>17881</v>
+    <row r="364" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="4">
+        <v>455</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C364" s="4">
+        <v>0</v>
+      </c>
+      <c r="D364" s="4">
+        <v>0</v>
+      </c>
+      <c r="E364" s="4">
+        <v>0</v>
+      </c>
+      <c r="F364" s="4">
+        <v>0</v>
+      </c>
+      <c r="G364" s="4">
+        <v>0</v>
+      </c>
+      <c r="H364" s="4">
+        <v>0</v>
+      </c>
+      <c r="I364" s="4">
+        <v>0</v>
+      </c>
+      <c r="J364" s="4">
+        <v>0</v>
+      </c>
+      <c r="K364" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="4">
+        <v>456</v>
+      </c>
+      <c r="B365" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C365" s="4">
+        <v>0</v>
+      </c>
+      <c r="D365" s="4">
+        <v>0</v>
+      </c>
+      <c r="E365" s="4">
+        <v>0</v>
+      </c>
+      <c r="F365" s="4">
+        <v>0</v>
+      </c>
+      <c r="G365" s="4">
+        <v>0</v>
+      </c>
+      <c r="H365" s="4">
+        <v>0</v>
+      </c>
+      <c r="I365" s="4">
+        <v>0</v>
+      </c>
+      <c r="J365" s="4">
+        <v>0</v>
+      </c>
+      <c r="K365" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="4">
+        <v>457</v>
+      </c>
+      <c r="B366" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C366" s="4">
+        <v>0</v>
+      </c>
+      <c r="D366" s="4">
+        <v>0</v>
+      </c>
+      <c r="E366" s="4">
+        <v>0</v>
+      </c>
+      <c r="F366" s="4">
+        <v>0</v>
+      </c>
+      <c r="G366" s="4">
+        <v>0</v>
+      </c>
+      <c r="H366" s="4">
+        <v>0</v>
+      </c>
+      <c r="I366" s="4">
+        <v>0</v>
+      </c>
+      <c r="J366" s="4">
+        <v>0</v>
+      </c>
+      <c r="K366" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A367">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B367" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C367">
         <v>0</v>
@@ -14523,45 +14529,45 @@
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A368">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B368" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="D368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="E368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="F368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="G368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="H368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="I368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="J368">
-        <v>0</v>
+        <v>17881</v>
       </c>
       <c r="K368">
-        <v>0</v>
+        <v>17881</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A369">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B369" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C369">
         <v>0</v>
@@ -14593,10 +14599,10 @@
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A370">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B370" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C370">
         <v>0</v>
@@ -14628,10 +14634,10 @@
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A371">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B371" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C371">
         <v>0</v>
@@ -14663,10 +14669,10 @@
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A372">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B372" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C372">
         <v>0</v>
@@ -14698,10 +14704,10 @@
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A373">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B373" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C373">
         <v>0</v>
@@ -14733,10 +14739,10 @@
     </row>
     <row r="374" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A374">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B374" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C374">
         <v>0</v>
@@ -14768,10 +14774,10 @@
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A375">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B375" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C375">
         <v>0</v>
@@ -14803,10 +14809,10 @@
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A376">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B376" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C376">
         <v>0</v>
@@ -14838,185 +14844,185 @@
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A377">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B377" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C377">
         <v>0</v>
       </c>
       <c r="D377">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E377">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="F377">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="G377">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="H377">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="I377">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="J377">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="K377">
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A378">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B378" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C378">
         <v>0</v>
       </c>
       <c r="D378">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="E378">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="F378">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="G378">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="H378">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="I378">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="J378">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="K378">
-        <v>269167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A379">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B379" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C379">
         <v>0</v>
       </c>
       <c r="D379">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="E379">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="F379">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="G379">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="H379">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="I379">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="J379">
-        <v>269167</v>
+        <v>110</v>
       </c>
       <c r="K379">
-        <v>269167</v>
+        <v>110</v>
       </c>
     </row>
     <row r="380" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A380">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B380" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C380">
         <v>0</v>
       </c>
       <c r="D380">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="E380">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="F380">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="G380">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="H380">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="I380">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="J380">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="K380">
-        <v>0</v>
+        <v>269167</v>
       </c>
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A381">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B381" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C381">
         <v>0</v>
       </c>
       <c r="D381">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="E381">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="F381">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="G381">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="H381">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="I381">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="J381">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="K381">
-        <v>0</v>
+        <v>269167</v>
       </c>
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A382">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B382" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C382">
         <v>0</v>
@@ -15048,80 +15054,80 @@
     </row>
     <row r="383" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A383">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B383" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C383">
         <v>0</v>
       </c>
       <c r="D383">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="E383">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="F383">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="G383">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="H383">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="I383">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="J383">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="K383">
-        <v>269167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A384">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B384" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C384">
         <v>0</v>
       </c>
       <c r="D384">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="E384">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="F384">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="G384">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="H384">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="I384">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="J384">
-        <v>269167</v>
+        <v>0</v>
       </c>
       <c r="K384">
-        <v>269167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A385">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B385" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C385">
         <v>0</v>
@@ -15153,115 +15159,115 @@
     </row>
     <row r="386" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A386">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B386" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C386">
         <v>0</v>
       </c>
       <c r="D386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="E386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="F386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="G386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="H386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="I386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="J386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
       <c r="K386">
-        <v>1103</v>
+        <v>269167</v>
       </c>
     </row>
     <row r="387" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A387">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B387" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C387">
         <v>0</v>
       </c>
       <c r="D387">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="E387">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="F387">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="G387">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="H387">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="I387">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="J387">
-        <v>0</v>
+        <v>269167</v>
       </c>
       <c r="K387">
-        <v>0</v>
+        <v>269167</v>
       </c>
     </row>
     <row r="388" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A388">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B388" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C388">
         <v>0</v>
       </c>
       <c r="D388">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="E388">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="F388">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="G388">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="H388">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="I388">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="J388">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="K388">
-        <v>0</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A389">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B389" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C389">
         <v>0</v>
@@ -15293,10 +15299,10 @@
     </row>
     <row r="390" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A390">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B390" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C390">
         <v>0</v>
@@ -15328,10 +15334,10 @@
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A391">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B391" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C391">
         <v>0</v>
@@ -15363,10 +15369,10 @@
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A392">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B392" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C392">
         <v>0</v>
@@ -15398,10 +15404,10 @@
     </row>
     <row r="393" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A393">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B393" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C393">
         <v>0</v>
@@ -15433,10 +15439,10 @@
     </row>
     <row r="394" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A394">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B394" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C394">
         <v>0</v>
@@ -15468,10 +15474,10 @@
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A395">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B395" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C395">
         <v>0</v>
@@ -15503,10 +15509,10 @@
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A396">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B396" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C396">
         <v>0</v>
@@ -15536,12 +15542,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A397">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B397" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C397">
         <v>0</v>
@@ -15573,220 +15579,220 @@
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A398">
+        <v>491</v>
+      </c>
+      <c r="B398" t="s">
+        <v>392</v>
+      </c>
+      <c r="C398">
+        <v>0</v>
+      </c>
+      <c r="D398">
+        <v>0</v>
+      </c>
+      <c r="E398">
+        <v>0</v>
+      </c>
+      <c r="F398">
+        <v>0</v>
+      </c>
+      <c r="G398">
+        <v>0</v>
+      </c>
+      <c r="H398">
+        <v>0</v>
+      </c>
+      <c r="I398">
+        <v>0</v>
+      </c>
+      <c r="J398">
+        <v>0</v>
+      </c>
+      <c r="K398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <v>492</v>
+      </c>
+      <c r="B399" t="s">
+        <v>393</v>
+      </c>
+      <c r="C399">
+        <v>0</v>
+      </c>
+      <c r="D399">
+        <v>0</v>
+      </c>
+      <c r="E399">
+        <v>0</v>
+      </c>
+      <c r="F399">
+        <v>0</v>
+      </c>
+      <c r="G399">
+        <v>0</v>
+      </c>
+      <c r="H399">
+        <v>0</v>
+      </c>
+      <c r="I399">
+        <v>0</v>
+      </c>
+      <c r="J399">
+        <v>0</v>
+      </c>
+      <c r="K399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A400">
         <v>494</v>
       </c>
-      <c r="B398" t="s">
-        <v>395</v>
-      </c>
-      <c r="C398">
-        <v>0</v>
-      </c>
-      <c r="D398">
+      <c r="B400" t="s">
+        <v>394</v>
+      </c>
+      <c r="C400">
+        <v>0</v>
+      </c>
+      <c r="D400">
         <v>6</v>
       </c>
-      <c r="E398">
+      <c r="E400">
         <v>6</v>
       </c>
-      <c r="F398">
+      <c r="F400">
         <v>6</v>
       </c>
-      <c r="G398">
+      <c r="G400">
         <v>6</v>
       </c>
-      <c r="H398">
+      <c r="H400">
         <v>6</v>
       </c>
-      <c r="I398">
+      <c r="I400">
         <v>6</v>
       </c>
-      <c r="J398">
+      <c r="J400">
         <v>6</v>
       </c>
-      <c r="K398">
+      <c r="K400">
         <v>6</v>
-      </c>
-    </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A399" s="4">
-        <v>496</v>
-      </c>
-      <c r="B399" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="C399" s="4">
-        <v>0</v>
-      </c>
-      <c r="D399" s="4">
-        <v>0</v>
-      </c>
-      <c r="E399" s="4">
-        <v>0</v>
-      </c>
-      <c r="F399" s="4">
-        <v>0</v>
-      </c>
-      <c r="G399" s="4">
-        <v>0</v>
-      </c>
-      <c r="H399" s="4">
-        <v>0</v>
-      </c>
-      <c r="I399" s="4">
-        <v>0</v>
-      </c>
-      <c r="J399" s="4">
-        <v>0</v>
-      </c>
-      <c r="K399" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A400" s="4">
-        <v>497</v>
-      </c>
-      <c r="B400" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="C400" s="4">
-        <v>0</v>
-      </c>
-      <c r="D400" s="4">
-        <v>0</v>
-      </c>
-      <c r="E400" s="4">
-        <v>0</v>
-      </c>
-      <c r="F400" s="4">
-        <v>0</v>
-      </c>
-      <c r="G400" s="4">
-        <v>0</v>
-      </c>
-      <c r="H400" s="4">
-        <v>0</v>
-      </c>
-      <c r="I400" s="4">
-        <v>0</v>
-      </c>
-      <c r="J400" s="4">
-        <v>0</v>
-      </c>
-      <c r="K400" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="401" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A401" s="4">
+        <v>496</v>
+      </c>
+      <c r="B401" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C401" s="4">
+        <v>0</v>
+      </c>
+      <c r="D401" s="4">
+        <v>0</v>
+      </c>
+      <c r="E401" s="4">
+        <v>0</v>
+      </c>
+      <c r="F401" s="4">
+        <v>0</v>
+      </c>
+      <c r="G401" s="4">
+        <v>0</v>
+      </c>
+      <c r="H401" s="4">
+        <v>0</v>
+      </c>
+      <c r="I401" s="4">
+        <v>0</v>
+      </c>
+      <c r="J401" s="4">
+        <v>0</v>
+      </c>
+      <c r="K401" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A402" s="4">
+        <v>497</v>
+      </c>
+      <c r="B402" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C402" s="4">
+        <v>0</v>
+      </c>
+      <c r="D402" s="4">
+        <v>0</v>
+      </c>
+      <c r="E402" s="4">
+        <v>0</v>
+      </c>
+      <c r="F402" s="4">
+        <v>0</v>
+      </c>
+      <c r="G402" s="4">
+        <v>0</v>
+      </c>
+      <c r="H402" s="4">
+        <v>0</v>
+      </c>
+      <c r="I402" s="4">
+        <v>0</v>
+      </c>
+      <c r="J402" s="4">
+        <v>0</v>
+      </c>
+      <c r="K402" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A403" s="4">
         <v>498</v>
       </c>
-      <c r="B401" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="C401" s="4">
-        <v>0</v>
-      </c>
-      <c r="D401" s="4">
-        <v>0</v>
-      </c>
-      <c r="E401" s="4">
-        <v>0</v>
-      </c>
-      <c r="F401" s="4">
-        <v>0</v>
-      </c>
-      <c r="G401" s="4">
-        <v>0</v>
-      </c>
-      <c r="H401" s="4">
-        <v>0</v>
-      </c>
-      <c r="I401" s="4">
-        <v>0</v>
-      </c>
-      <c r="J401" s="4">
-        <v>0</v>
-      </c>
-      <c r="K401" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="402" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A402">
+      <c r="B403" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C403" s="4">
+        <v>0</v>
+      </c>
+      <c r="D403" s="4">
+        <v>0</v>
+      </c>
+      <c r="E403" s="4">
+        <v>0</v>
+      </c>
+      <c r="F403" s="4">
+        <v>0</v>
+      </c>
+      <c r="G403" s="4">
+        <v>0</v>
+      </c>
+      <c r="H403" s="4">
+        <v>0</v>
+      </c>
+      <c r="I403" s="4">
+        <v>0</v>
+      </c>
+      <c r="J403" s="4">
+        <v>0</v>
+      </c>
+      <c r="K403" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A404">
         <v>500</v>
       </c>
-      <c r="B402" t="s">
-        <v>396</v>
-      </c>
-      <c r="C402">
-        <v>0</v>
-      </c>
-      <c r="D402">
-        <v>0</v>
-      </c>
-      <c r="E402">
-        <v>0</v>
-      </c>
-      <c r="F402">
-        <v>0</v>
-      </c>
-      <c r="G402">
-        <v>0</v>
-      </c>
-      <c r="H402">
-        <v>0</v>
-      </c>
-      <c r="I402">
-        <v>0</v>
-      </c>
-      <c r="J402">
-        <v>0</v>
-      </c>
-      <c r="K402">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A403">
-        <v>501</v>
-      </c>
-      <c r="B403" t="s">
-        <v>397</v>
-      </c>
-      <c r="C403">
-        <v>0</v>
-      </c>
-      <c r="D403">
-        <v>0</v>
-      </c>
-      <c r="E403">
-        <v>0</v>
-      </c>
-      <c r="F403">
-        <v>0</v>
-      </c>
-      <c r="G403">
-        <v>0</v>
-      </c>
-      <c r="H403">
-        <v>0</v>
-      </c>
-      <c r="I403">
-        <v>0</v>
-      </c>
-      <c r="J403">
-        <v>0</v>
-      </c>
-      <c r="K403">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A404">
-        <v>503</v>
-      </c>
       <c r="B404" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C404">
         <v>0</v>
@@ -15818,10 +15824,10 @@
     </row>
     <row r="405" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A405">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B405" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C405">
         <v>0</v>
@@ -15853,10 +15859,10 @@
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A406">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B406" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C406">
         <v>0</v>
@@ -15888,141 +15894,211 @@
     </row>
     <row r="407" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A407">
+        <v>504</v>
+      </c>
+      <c r="B407" t="s">
+        <v>398</v>
+      </c>
+      <c r="C407">
+        <v>0</v>
+      </c>
+      <c r="D407">
+        <v>0</v>
+      </c>
+      <c r="E407">
+        <v>0</v>
+      </c>
+      <c r="F407">
+        <v>0</v>
+      </c>
+      <c r="G407">
+        <v>0</v>
+      </c>
+      <c r="H407">
+        <v>0</v>
+      </c>
+      <c r="I407">
+        <v>0</v>
+      </c>
+      <c r="J407">
+        <v>0</v>
+      </c>
+      <c r="K407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>505</v>
+      </c>
+      <c r="B408" t="s">
+        <v>399</v>
+      </c>
+      <c r="C408">
+        <v>0</v>
+      </c>
+      <c r="D408">
+        <v>0</v>
+      </c>
+      <c r="E408">
+        <v>0</v>
+      </c>
+      <c r="F408">
+        <v>0</v>
+      </c>
+      <c r="G408">
+        <v>0</v>
+      </c>
+      <c r="H408">
+        <v>0</v>
+      </c>
+      <c r="I408">
+        <v>0</v>
+      </c>
+      <c r="J408">
+        <v>0</v>
+      </c>
+      <c r="K408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A409">
         <v>506</v>
       </c>
-      <c r="B407" t="s">
-        <v>401</v>
-      </c>
-      <c r="C407">
-        <v>0</v>
-      </c>
-      <c r="D407">
-        <v>0</v>
-      </c>
-      <c r="E407">
-        <v>0</v>
-      </c>
-      <c r="F407">
-        <v>0</v>
-      </c>
-      <c r="G407">
-        <v>0</v>
-      </c>
-      <c r="H407">
-        <v>0</v>
-      </c>
-      <c r="I407">
-        <v>0</v>
-      </c>
-      <c r="J407">
-        <v>0</v>
-      </c>
-      <c r="K407">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A408" s="4">
-        <v>507</v>
-      </c>
-      <c r="B408" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="C408" s="4">
-        <v>0</v>
-      </c>
-      <c r="D408" s="4">
-        <v>0</v>
-      </c>
-      <c r="E408" s="4">
-        <v>0</v>
-      </c>
-      <c r="F408" s="4">
-        <v>0</v>
-      </c>
-      <c r="G408" s="4">
-        <v>0</v>
-      </c>
-      <c r="H408" s="4">
-        <v>0</v>
-      </c>
-      <c r="I408" s="4">
-        <v>0</v>
-      </c>
-      <c r="J408" s="4">
-        <v>0</v>
-      </c>
-      <c r="K408" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A409" s="4">
-        <v>508</v>
-      </c>
-      <c r="B409" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="C409" s="4">
-        <v>0</v>
-      </c>
-      <c r="D409" s="4">
-        <v>0</v>
-      </c>
-      <c r="E409" s="4">
-        <v>0</v>
-      </c>
-      <c r="F409" s="4">
-        <v>0</v>
-      </c>
-      <c r="G409" s="4">
-        <v>0</v>
-      </c>
-      <c r="H409" s="4">
-        <v>0</v>
-      </c>
-      <c r="I409" s="4">
-        <v>0</v>
-      </c>
-      <c r="J409" s="4">
-        <v>0</v>
-      </c>
-      <c r="K409" s="4">
+      <c r="B409" t="s">
+        <v>400</v>
+      </c>
+      <c r="C409">
+        <v>0</v>
+      </c>
+      <c r="D409">
+        <v>0</v>
+      </c>
+      <c r="E409">
+        <v>0</v>
+      </c>
+      <c r="F409">
+        <v>0</v>
+      </c>
+      <c r="G409">
+        <v>0</v>
+      </c>
+      <c r="H409">
+        <v>0</v>
+      </c>
+      <c r="I409">
+        <v>0</v>
+      </c>
+      <c r="J409">
+        <v>0</v>
+      </c>
+      <c r="K409">
         <v>0</v>
       </c>
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A410" s="4">
+        <v>507</v>
+      </c>
+      <c r="B410" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C410" s="4">
+        <v>0</v>
+      </c>
+      <c r="D410" s="4">
+        <v>0</v>
+      </c>
+      <c r="E410" s="4">
+        <v>0</v>
+      </c>
+      <c r="F410" s="4">
+        <v>0</v>
+      </c>
+      <c r="G410" s="4">
+        <v>0</v>
+      </c>
+      <c r="H410" s="4">
+        <v>0</v>
+      </c>
+      <c r="I410" s="4">
+        <v>0</v>
+      </c>
+      <c r="J410" s="4">
+        <v>0</v>
+      </c>
+      <c r="K410" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A411" s="4">
+        <v>508</v>
+      </c>
+      <c r="B411" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C411" s="4">
+        <v>0</v>
+      </c>
+      <c r="D411" s="4">
+        <v>0</v>
+      </c>
+      <c r="E411" s="4">
+        <v>0</v>
+      </c>
+      <c r="F411" s="4">
+        <v>0</v>
+      </c>
+      <c r="G411" s="4">
+        <v>0</v>
+      </c>
+      <c r="H411" s="4">
+        <v>0</v>
+      </c>
+      <c r="I411" s="4">
+        <v>0</v>
+      </c>
+      <c r="J411" s="4">
+        <v>0</v>
+      </c>
+      <c r="K411" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A412" s="4">
         <v>509</v>
       </c>
-      <c r="B410" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="C410" s="4">
-        <v>0</v>
-      </c>
-      <c r="D410" s="4">
-        <v>0</v>
-      </c>
-      <c r="E410" s="4">
-        <v>0</v>
-      </c>
-      <c r="F410" s="4">
-        <v>0</v>
-      </c>
-      <c r="G410" s="4">
-        <v>0</v>
-      </c>
-      <c r="H410" s="4">
-        <v>0</v>
-      </c>
-      <c r="I410" s="4">
-        <v>0</v>
-      </c>
-      <c r="J410" s="4">
-        <v>0</v>
-      </c>
-      <c r="K410" s="4">
+      <c r="B412" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C412" s="4">
+        <v>0</v>
+      </c>
+      <c r="D412" s="4">
+        <v>0</v>
+      </c>
+      <c r="E412" s="4">
+        <v>0</v>
+      </c>
+      <c r="F412" s="4">
+        <v>0</v>
+      </c>
+      <c r="G412" s="4">
+        <v>0</v>
+      </c>
+      <c r="H412" s="4">
+        <v>0</v>
+      </c>
+      <c r="I412" s="4">
+        <v>0</v>
+      </c>
+      <c r="J412" s="4">
+        <v>0</v>
+      </c>
+      <c r="K412" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>